<commit_message>
Update Excel template and add lock file for PLK; limit Excel row processing to 200
</commit_message>
<xml_diff>
--- a/workplace/jobs/qt_autogen/excel_templates/template_PLK.xlsx
+++ b/workplace/jobs/qt_autogen/excel_templates/template_PLK.xlsx
@@ -11,7 +11,7 @@
     <sheet name="ฟอร์มราคา-ใช้ sheet นี้ทำQT" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ฟอร์มราคา-ใช้ sheet นี้ทำQT'!$A$1:$K$68</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'ฟอร์มราคา-ใช้ sheet นี้ทำQT'!$A:$K</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t xml:space="preserve">ใบเสนอราคา</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cost price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">รายการ New Code</t>
   </si>
   <si>
     <t xml:space="preserve">เงื่อนไข: </t>
@@ -146,7 +143,7 @@
     <numFmt numFmtId="169" formatCode="#,##0"/>
     <numFmt numFmtId="170" formatCode="0;[RED]0"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="14"/>
       <name val="Cordia New"/>
@@ -399,23 +396,31 @@
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Angsana New"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Angsana New"/>
-      <family val="1"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="26"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <color rgb="FF000000"/>
       <name val="Angsana New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="32"/>
-      <name val="Angsana New"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="36">
@@ -979,167 +984,167 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="33" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="33" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="33" fillId="33" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="33" fillId="33" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="34" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="34" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="33" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="34" fillId="35" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="34" fillId="35" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1208,23 +1213,6 @@
     <cellStyle name="Warning Text 2" xfId="74"/>
     <cellStyle name="ปกติ 3 2" xfId="75"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC0C0C0"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1294,14 +1282,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>907200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>628920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>364680</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
+      <xdr:colOff>363960</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1310,8 +1298,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13686120" y="18961200"/>
-          <a:ext cx="9908280" cy="3405240"/>
+          <a:off x="13683960" y="17463960"/>
+          <a:ext cx="9905760" cy="3404520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1333,7 +1321,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" anchor="ctr" upright="1">
+        <a:bodyPr vertOverflow="clip" lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="ctr" upright="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1413,6 +1401,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>(Jantharat  Krainara ) </a:t>
@@ -1420,6 +1411,9 @@
           <a:br/>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>Senior Manager, Business Advancement</a:t>
@@ -1436,6 +1430,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>Date: 25 / 07 / 2025</a:t>
@@ -1452,14 +1449,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>675000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1312200</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:colOff>1311480</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1468,8 +1465,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5545440" y="22615200"/>
-          <a:ext cx="13713120" cy="4039920"/>
+          <a:off x="5544360" y="21117960"/>
+          <a:ext cx="13710240" cy="4038840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1491,7 +1488,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" anchor="ctr" upright="1">
+        <a:bodyPr vertOverflow="clip" lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="ctr" upright="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1607,6 +1604,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>------------------------------------------------</a:t>
@@ -1626,12 +1626,18 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>( </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" lang="th-TH" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
               <a:cs typeface="Angsana New"/>
             </a:rPr>
@@ -1639,6 +1645,9 @@
           </a:r>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>)</a:t>
@@ -1658,6 +1667,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="th-TH" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
               <a:cs typeface="Angsana New"/>
             </a:rPr>
@@ -1665,12 +1677,18 @@
           </a:r>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>- </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" lang="th-TH" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
               <a:cs typeface="Angsana New"/>
             </a:rPr>
@@ -1691,12 +1709,18 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>Date: …... / …..../ …….  </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="3200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>           </a:t>
@@ -1713,14 +1737,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>590400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>638280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1005840</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:colOff>1005120</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1729,8 +1753,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1415880" y="18970560"/>
-          <a:ext cx="10453680" cy="3396600"/>
+          <a:off x="1415160" y="17473320"/>
+          <a:ext cx="10452240" cy="3395880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1752,7 +1776,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" anchor="ctr" upright="1">
+        <a:bodyPr vertOverflow="clip" lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="ctr" upright="1">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1832,6 +1856,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>(Potjanee Kanchaiyaphum)                                       </a:t>
@@ -1848,12 +1875,18 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t> </a:t>
           </a:r>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>Key Account Executive - Paolo group </a:t>
@@ -1870,6 +1903,9 @@
           </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="2600" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Angsana New"/>
             </a:rPr>
             <a:t>Date: 25 / 07 / 2025</a:t>
@@ -1886,14 +1922,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>914400</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1499040</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:colOff>1498320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>388080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1906,8 +1942,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17440920" y="19904040"/>
-          <a:ext cx="2004480" cy="760320"/>
+          <a:off x="17438400" y="17671320"/>
+          <a:ext cx="2003040" cy="1495080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1923,14 +1959,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>102960</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>931680</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2666880</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>312480</xdr:rowOff>
+      <xdr:colOff>2666160</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1943,8 +1979,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4973400" y="19921320"/>
-          <a:ext cx="2563920" cy="1149840"/>
+          <a:off x="4972320" y="17671320"/>
+          <a:ext cx="2563200" cy="1149120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2141,11 +2177,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23:K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.078125" defaultRowHeight="35.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.5"/>
@@ -2175,7 +2211,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" s="6" customFormat="true" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="6" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2352,165 +2388,165 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" s="23" customFormat="true" ht="51.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
-        <v>22</v>
-      </c>
+    <row r="13" s="23" customFormat="true" ht="51.35" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24"/>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="25"/>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" s="23" customFormat="true" ht="86.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="25"/>
+    <row r="14" s="23" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="28"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-    </row>
-    <row r="15" s="30" customFormat="true" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" s="32" customFormat="true" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="29" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-    </row>
-    <row r="16" s="30" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32" t="s">
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" s="32" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-    </row>
-    <row r="17" s="30" customFormat="true" ht="51.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" s="32" customFormat="true" ht="51.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-    </row>
-    <row r="18" s="30" customFormat="true" ht="51.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35" t="s">
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" s="32" customFormat="true" ht="51.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-    </row>
-    <row r="19" s="30" customFormat="true" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" s="32" customFormat="true" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-    </row>
-    <row r="20" s="30" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
+      <c r="B19" s="35"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="36" t="s">
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" s="32" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" s="32" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" s="32" customFormat="true" ht="385.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-    </row>
-    <row r="21" s="30" customFormat="true" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-    </row>
-    <row r="22" s="30" customFormat="true" ht="385.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36"/>
       <c r="B22" s="36"/>
-      <c r="C22" s="34"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="36"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-    </row>
-    <row r="23" s="33" customFormat="true" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+    </row>
+    <row r="23" s="31" customFormat="true" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
         <v>33</v>
       </c>
@@ -2525,56 +2561,54 @@
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
     </row>
-    <row r="24" s="33" customFormat="true" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" s="33" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
+    <row r="24" s="31" customFormat="true" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" s="31" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" s="33" customFormat="true" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
+    <row r="26" s="31" customFormat="true" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="2"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" s="33" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="31" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2593,10 +2627,10 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" s="41" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="40"/>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -2605,19 +2639,25 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-    </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C32" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2626,19 +2666,29 @@
     <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="12.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="14">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:D3"/>
@@ -2653,10 +2703,6 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>